<commit_message>
Pushing pending changes to plots_for_eda.xlsx
</commit_message>
<xml_diff>
--- a/plots_for_eda.xlsx
+++ b/plots_for_eda.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\BerkeleyMIDS\projects\w207_final_project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C98D2052-DB4D-4C36-AA21-130A3E5E619D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01300D6F-3A12-4AD6-BE26-E5E049B501AE}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{809DF9D7-308F-4863-90B9-1D16096864B3}"/>
   </bookViews>
@@ -121,12 +121,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -141,7 +147,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -150,12 +156,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFC000"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -441,7 +453,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{238FDFA5-99A1-4612-B47A-EE61C775F175}" type="CELLRANGE">
+                    <a:fld id="{23ABDB50-B5EE-4585-A578-C6579CB38113}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -521,7 +533,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7537C695-F759-45A1-AA30-29BFEB5646C5}" type="CELLRANGE">
+                    <a:fld id="{72759742-3EBD-4139-ACAA-516F0983A8FD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -601,7 +613,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{09460312-FC6D-4E97-935A-DC8BF75C7A14}" type="CELLRANGE">
+                    <a:fld id="{C2A49602-D870-415F-8E7B-A870C890BE2B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -681,7 +693,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{51D15937-E126-4503-998B-33B0CA5043B3}" type="CELLRANGE">
+                    <a:fld id="{FBC57B2C-3006-483D-BD3C-F9B2DD7F0C9B}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -761,7 +773,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{185BE104-5A16-430A-A7A9-D291BAA67537}" type="CELLRANGE">
+                    <a:fld id="{4FA088D3-6121-40AD-9A78-2038BBBA2EE8}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -841,7 +853,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{5979F711-CD60-49EE-B2BB-DC8828684D4A}" type="CELLRANGE">
+                    <a:fld id="{0397BE1F-1B11-482E-861E-0F9555C633D3}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -921,7 +933,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{41FD1E2E-4C58-4F57-A2D8-8ADCDCBF0A67}" type="CELLRANGE">
+                    <a:fld id="{266E34EF-30F4-41C0-B57F-A67607E4D384}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -1001,7 +1013,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{37A480EA-E11E-453B-BA02-523057C26C7B}" type="CELLRANGE">
+                    <a:fld id="{FF13BB4B-F931-4753-A4DC-5206C7CBE795}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -1081,7 +1093,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{ABDC08F9-0C86-45C5-A8E0-5E70629874DA}" type="CELLRANGE">
+                    <a:fld id="{83FF84E0-167A-4DBB-84E5-2FC0A7148CBD}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -1198,7 +1210,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{E17E3F7B-0B9A-409B-89FD-F8A0E950BC79}" type="CELLRANGE">
+                    <a:fld id="{EFFB4A7A-B951-4B7E-97A1-5F9EDBC76958}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -1266,7 +1278,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{66927811-787A-4F33-9840-713A28A0E730}" type="CELLRANGE">
+                    <a:fld id="{1947F059-DF4D-4C6A-A44B-1D54B0BF1B55}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -1686,6 +1698,25 @@
               </c:ext>
             </c:extLst>
           </c:dPt>
+          <c:dPt>
+            <c:idx val="11"/>
+            <c:invertIfNegative val="0"/>
+            <c:bubble3D val="0"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FFC000"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:extLst>
+              <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                <c16:uniqueId val="{0000000E-E31E-4906-A8A6-4E17F4010AE3}"/>
+              </c:ext>
+            </c:extLst>
+          </c:dPt>
           <c:cat>
             <c:multiLvlStrRef>
               <c:f>Sheet1!$E$10:$F$21</c:f>
@@ -1856,7 +1887,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{6CF2247A-ACBE-41E5-96FE-C5B8935D7B8E}" type="CELLRANGE">
+                    <a:fld id="{C88B4615-373E-4D26-875C-4C63C3FF6401}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -1934,7 +1965,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{9259A633-766E-4E7A-99E5-2255A2132F5F}" type="CELLRANGE">
+                    <a:fld id="{DB728DDA-F90E-4B4E-9700-B5BD6BA6E628}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2012,7 +2043,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7957D353-A141-446C-B83A-1FE4E597B97C}" type="CELLRANGE">
+                    <a:fld id="{FC5F7B2B-64A0-4A0D-A380-7162FC93BDE9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2090,7 +2121,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7EBDAF3F-5250-439A-B3D7-CC582C7AB71B}" type="CELLRANGE">
+                    <a:fld id="{B44E606E-26CB-4D85-917C-9BB668A74298}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2168,7 +2199,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{7BACD3D9-A6F6-4606-8BE3-710991265F0F}" type="CELLRANGE">
+                    <a:fld id="{A494C0B1-51F0-4C93-9D36-EBFF6B6DD0BC}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2246,7 +2277,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{881A4B91-44B5-4349-9CA8-7292E822AC84}" type="CELLRANGE">
+                    <a:fld id="{59A756AB-D305-40BE-ACEB-A44CC3908C19}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2324,7 +2355,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{0B63037D-C279-48DD-BA9D-23FABBAD9263}" type="CELLRANGE">
+                    <a:fld id="{BA5AFBEA-E9FA-4F8C-8E9D-AABC84564C9D}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2402,7 +2433,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{1C3ABB86-6F05-48EB-B3E9-1A320B7837EA}" type="CELLRANGE">
+                    <a:fld id="{FCDE635D-C40A-4E3F-9815-CB224BC1F341}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2480,7 +2511,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{8830DE25-49CD-443E-8D3B-7AA064A99FE7}" type="CELLRANGE">
+                    <a:fld id="{DCB480B5-3F94-4251-B008-8F6D9475E335}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2558,7 +2589,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{D4DFB159-A0FB-4A2A-9142-2AFBD36650C4}" type="CELLRANGE">
+                    <a:fld id="{99F56F27-8844-47D1-AAA2-AB260779329A}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2636,7 +2667,7 @@
                         <a:cs typeface="+mn-cs"/>
                       </a:defRPr>
                     </a:pPr>
-                    <a:fld id="{80D75CFF-D0F9-4BC1-9DB0-C0AE524EA004}" type="CELLRANGE">
+                    <a:fld id="{3044A53B-C5FD-444D-96E7-BB60DE63A620}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr>
                         <a:defRPr sz="1600">
@@ -2702,7 +2733,7 @@
                   <a:bodyPr/>
                   <a:lstStyle/>
                   <a:p>
-                    <a:fld id="{D07A779F-B1C2-4E47-9FB8-206A16B844A4}" type="CELLRANGE">
+                    <a:fld id="{66D3FC33-3472-4861-BE07-34225279E3F9}" type="CELLRANGE">
                       <a:rPr lang="en-US"/>
                       <a:pPr/>
                       <a:t>[CELLRANGE]</a:t>
@@ -3645,7 +3676,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" xr:uid="{4D3D8015-B2DB-434A-A492-C2AD53235794}">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="94" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -3842,7 +3873,7 @@
           </a:r>
           <a:r>
             <a:rPr lang="en-US" sz="1600" b="1" baseline="0"/>
-            <a:t> are moderately suggestive of categories 1, 2, 5</a:t>
+            <a:t> are moderately suggestive of categories 1, 2, 5, and 7</a:t>
           </a:r>
           <a:endParaRPr lang="en-US" sz="1600" b="1"/>
         </a:p>
@@ -4383,10 +4414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{30C4B624-734E-4D28-B4EA-CF4B211985B6}">
-  <dimension ref="C9:P21"/>
+  <dimension ref="C9:S23"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="O22" sqref="O22"/>
+    <sheetView topLeftCell="D15" workbookViewId="0">
+      <selection activeCell="Q24" sqref="Q24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4731,7 +4762,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="17" spans="3:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="17" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C17">
         <v>5000</v>
       </c>
@@ -4773,7 +4804,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="18" spans="3:16" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="3:19" ht="30" x14ac:dyDescent="0.25">
       <c r="C18">
         <v>3500</v>
       </c>
@@ -4815,7 +4846,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="19" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="19" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C19">
         <v>6500</v>
       </c>
@@ -4859,7 +4890,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="20" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="20" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C20">
         <v>6000</v>
       </c>
@@ -4903,7 +4934,7 @@
         <v>4000</v>
       </c>
     </row>
-    <row r="21" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="21" spans="3:19" x14ac:dyDescent="0.25">
       <c r="C21">
         <v>0</v>
       </c>
@@ -4945,6 +4976,32 @@
       </c>
       <c r="P21">
         <v>4000</v>
+      </c>
+    </row>
+    <row r="22" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="O22" s="4"/>
+      <c r="Q22">
+        <v>186</v>
+      </c>
+      <c r="R22">
+        <v>12</v>
+      </c>
+      <c r="S22">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="23" spans="3:19" x14ac:dyDescent="0.25">
+      <c r="Q23">
+        <f>Q22/255</f>
+        <v>0.72941176470588232</v>
+      </c>
+      <c r="R23">
+        <f>R22/255</f>
+        <v>4.7058823529411764E-2</v>
+      </c>
+      <c r="S23">
+        <f>S22/255</f>
+        <v>0.18431372549019609</v>
       </c>
     </row>
   </sheetData>

</xml_diff>